<commit_message>
Adjusted the styles of the input boxes
</commit_message>
<xml_diff>
--- a/tracker/logs/phish_results.xlsx
+++ b/tracker/logs/phish_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,6 +487,28 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>test@test.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>127.0.0.1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/139.0.0.0 Safari/537.36 Edg/139.0.0.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-08-22T09:59:40.556063+00:00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>